<commit_message>
start working to the pricing model
</commit_message>
<xml_diff>
--- a/docs/pricing-model.xlsx
+++ b/docs/pricing-model.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boyerje/Documents/Code/AWS/big-data-tenant-analytics/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A641CF3B-DA29-F546-8FBD-186EF6DF4CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE9DE93-95E7-4145-BFF8-A381E9743C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
+    <workbookView xWindow="420" yWindow="500" windowWidth="29460" windowHeight="10360" activeTab="1" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
-    <sheet name="GuardDuty" sheetId="2" r:id="rId2"/>
-    <sheet name="Lambda" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="S3" sheetId="7" r:id="rId2"/>
+    <sheet name="EKS" sheetId="8" r:id="rId3"/>
+    <sheet name="GuardDuty" sheetId="2" r:id="rId4"/>
+    <sheet name="Lambda" sheetId="3" r:id="rId5"/>
+    <sheet name="RDS-Postgresql" sheetId="4" r:id="rId6"/>
+    <sheet name="API Gateway" sheetId="6" r:id="rId7"/>
+    <sheet name="DynamoDB" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="136">
   <si>
     <t>nb-of-tenants</t>
   </si>
@@ -50,15 +54,9 @@
     <t>QuickSight</t>
   </si>
   <si>
-    <t>nb-of-users-dev</t>
-  </si>
-  <si>
     <t>Average data set size per job</t>
   </si>
   <si>
-    <t>nb-of-job/day/dev</t>
-  </si>
-  <si>
     <t>guardduty</t>
   </si>
   <si>
@@ -143,28 +141,329 @@
     <t>K</t>
   </si>
   <si>
-    <t xml:space="preserve">Incoming Sagemaker API calls </t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Pricing</t>
   </si>
   <si>
     <t>per M request</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incoming Lambda/Sagemaker API calls </t>
+  </si>
+  <si>
+    <t>DynamoDB</t>
+  </si>
+  <si>
+    <t>Per WCU per hour</t>
+  </si>
+  <si>
+    <t>Per RCU per hour</t>
+  </si>
+  <si>
+    <t>Per GB storage per month</t>
+  </si>
+  <si>
+    <t>Point-in-time recovery, per GB per month</t>
+  </si>
+  <si>
+    <t>Replication WCU per hour</t>
+  </si>
+  <si>
+    <t>egress per GB over DX</t>
+  </si>
+  <si>
+    <t>Writes per month</t>
+  </si>
+  <si>
+    <t>Reads per month</t>
+  </si>
+  <si>
+    <t>Item size (KB)</t>
+  </si>
+  <si>
+    <t>Storage (GB)</t>
+  </si>
+  <si>
+    <t>RCU required</t>
+  </si>
+  <si>
+    <t>WCU required</t>
+  </si>
+  <si>
+    <t>WCU</t>
+  </si>
+  <si>
+    <t>RCU</t>
+  </si>
+  <si>
+    <t>PITR</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>RDS PostgreSQL - write ops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DynamoDB Writes ops </t>
+  </si>
+  <si>
+    <t>RDS PostgreSQL - Read ops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenant creation, update, churn update, # job 30 and 90 </t>
+  </si>
+  <si>
+    <t>4 times the writes numbers</t>
+  </si>
+  <si>
+    <t>Events on job submissions, cancel or termination</t>
+  </si>
+  <si>
+    <t>nb-of-job/day/developer</t>
+  </si>
+  <si>
+    <t>nb-of-user-developer overall</t>
+  </si>
+  <si>
+    <t>RDS</t>
+  </si>
+  <si>
+    <t>per hour</t>
+  </si>
+  <si>
+    <t>1 Region - Multi AZ - one standby</t>
+  </si>
+  <si>
+    <t>On-demand</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>up front</t>
+  </si>
+  <si>
+    <t>GB/month</t>
+  </si>
+  <si>
+    <t>Multi AZ - Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO Rate / </t>
+  </si>
+  <si>
+    <t>IOPS month</t>
+  </si>
+  <si>
+    <t>Write operation</t>
+  </si>
+  <si>
+    <t>Read operation</t>
+  </si>
+  <si>
+    <t>IOPS</t>
+  </si>
+  <si>
+    <t>per sec</t>
+  </si>
+  <si>
+    <t>nb-h-work-day</t>
+  </si>
+  <si>
+    <t># working day</t>
+  </si>
+  <si>
+    <t>Storage total</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>API Gateway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per 1M requests </t>
+  </si>
+  <si>
+    <t>first 333 M</t>
+  </si>
+  <si>
+    <t>next 667 M</t>
+  </si>
+  <si>
+    <t>next 19 B</t>
+  </si>
+  <si>
+    <t>over 20 B</t>
+  </si>
+  <si>
+    <t>Caching per hour</t>
+  </si>
+  <si>
+    <t>Transfer out per GB (DX)</t>
+  </si>
+  <si>
+    <t>Number of API calls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                              -  </t>
+  </si>
+  <si>
+    <t>Cache usage (GB)</t>
+  </si>
+  <si>
+    <t>Cache size (GB)</t>
+  </si>
+  <si>
+    <t>Cache cost per hour</t>
+  </si>
+  <si>
+    <t>Egress (GB)</t>
+  </si>
+  <si>
+    <t>API calls</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>Egress</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>% Utilization</t>
+  </si>
+  <si>
+    <t>Backup Storage</t>
+  </si>
+  <si>
+    <t>Backup storage</t>
+  </si>
+  <si>
+    <t>Backup</t>
+  </si>
+  <si>
+    <t>db.m1.large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthly at </t>
+  </si>
+  <si>
+    <t>utilization</t>
+  </si>
+  <si>
+    <t>RDS Proxy</t>
+  </si>
+  <si>
+    <t>RDS proxy (2VCPU)</t>
+  </si>
+  <si>
+    <t>EKS (EC2)</t>
+  </si>
+  <si>
+    <t>instance per hour (m4.2xlarge, RI)</t>
+  </si>
+  <si>
+    <t>Control plane per hour</t>
+  </si>
+  <si>
+    <t>per ALB hour</t>
+  </si>
+  <si>
+    <t>per ALB LCU hour</t>
+  </si>
+  <si>
+    <t>per EBS GB per month</t>
+  </si>
+  <si>
+    <t>Monthly API calls</t>
+  </si>
+  <si>
+    <t>CPU-per-GB ratio</t>
+  </si>
+  <si>
+    <t>LCUs (connections per second)</t>
+  </si>
+  <si>
+    <t>API calls per second</t>
+  </si>
+  <si>
+    <t>Max API calls in flight concurrently</t>
+  </si>
+  <si>
+    <t>Concurrent RAM necessary</t>
+  </si>
+  <si>
+    <t>Concurrent CPU necessary</t>
+  </si>
+  <si>
+    <t>EBS volume size (GB)</t>
+  </si>
+  <si>
+    <t>CPU per instance</t>
+  </si>
+  <si>
+    <t>RAM per instance</t>
+  </si>
+  <si>
+    <t>Number of instances required</t>
+  </si>
+  <si>
+    <t>Instances</t>
+  </si>
+  <si>
+    <t>Control plane</t>
+  </si>
+  <si>
+    <t>ELB</t>
+  </si>
+  <si>
+    <t>EBS</t>
+  </si>
+  <si>
+    <t>Average data size</t>
+  </si>
+  <si>
+    <t>Replication factors - due to user</t>
+  </si>
+  <si>
+    <t>Big-data user's data size - overall with all tenant</t>
+  </si>
+  <si>
+    <t>Overall storage cross tenants</t>
+  </si>
+  <si>
+    <t>&gt; 500 TB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50 to 500 TB</t>
+  </si>
+  <si>
+    <t>First 50 TB / Month</t>
+  </si>
+  <si>
+    <t>TB / month</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="7">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0000_);[Red]\(&quot;$&quot;#,##0.0000\)"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,6 +509,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF16191F"/>
+      <name val="Amazon Ember"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -225,7 +580,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -253,37 +608,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF4472C4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF4472C4"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF4472C4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="5" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Title" xfId="2" builtinId="15"/>
-    <cellStyle name="Total" xfId="4" builtinId="25"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Title" xfId="3" builtinId="15"/>
+    <cellStyle name="Total" xfId="5" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -595,54 +1001,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34F96F2-6121-1F44-9B56-6D7ABA1B499B}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="B4">
         <f>B3*10</f>
         <v>5000</v>
       </c>
+      <c r="C4" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4">
+        <v>1.7</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="9">
+        <v>59</v>
+      </c>
+      <c r="B5" s="8">
         <v>2.7</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>32</v>
+      <c r="D5" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="E5">
         <f>2*B5</f>
@@ -651,9 +1075,9 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
         <v>1000</v>
       </c>
       <c r="C6" t="s">
@@ -662,101 +1086,189 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="9">
+        <v>20</v>
+      </c>
+      <c r="B7" s="8">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="9">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8">
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="8">
+        <f>B3*D3*D4</f>
+        <v>85000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B13">
-        <f>B4/2*$B$5</f>
+      <c r="B16">
+        <f>$B$4/2*$B$5</f>
         <v>6750</v>
       </c>
-      <c r="C13">
-        <f>B13*20</f>
+      <c r="C16">
+        <f>B16*20</f>
         <v>135000</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17">
+        <f>B16+B3/2</f>
+        <v>7000</v>
+      </c>
+      <c r="C17">
+        <f>B17*20</f>
+        <v>140000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18">
+        <f>B17*4</f>
+        <v>28000</v>
+      </c>
+      <c r="C18">
+        <f>B18*20</f>
+        <v>560000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <f>$B$4/2*$B$5*2</f>
+        <v>13500</v>
+      </c>
+      <c r="C19">
+        <f>B19*20</f>
+        <v>270000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="10">
+        <f>Lambda!B15</f>
+        <v>5.0905125000000009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="10">
+        <f>'RDS-Postgresql'!B28</f>
+        <v>501.2374999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>30</v>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="10">
+        <f>DynamoDB!B25</f>
+        <v>1.5760296386718751</v>
       </c>
     </row>
   </sheetData>
@@ -765,6 +1277,321 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D75016-8D7E-6241-A9EC-C6A4879139F1}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="31">
+        <v>2.3E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="13"/>
+    </row>
+    <row r="11" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11">
+        <f>Assumptions!B10</f>
+        <v>85000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17">
+        <f>(B11-50000)</f>
+        <v>35000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C681A54-95E7-4345-B314-53EA192E29AF}">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="18"/>
+    </row>
+    <row r="10" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="13"/>
+    </row>
+    <row r="11" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="17">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="17">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="17">
+        <v>3.09</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="17">
+        <v>30.86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="17">
+        <v>23.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="17">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="13"/>
+    </row>
+    <row r="24" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="18">
+        <v>108.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="18">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="18">
+        <v>33.979999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="19">
+        <v>296.27999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4E1C13-7392-0E41-A5F4-7D1FC3F71AD2}">
   <dimension ref="A3"/>
   <sheetViews>
@@ -776,7 +1603,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -787,12 +1614,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098A98AF-AD43-C846-A6AB-538EEBD2CE08}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,21 +1630,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -825,7 +1652,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4">
         <v>1.6670000000000001E-5</v>
@@ -833,22 +1660,22 @@
     </row>
     <row r="7" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5">
-        <f>Assumptions!C13</f>
+        <f>Assumptions!C16</f>
         <v>135000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -856,7 +1683,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0.75</v>
@@ -864,25 +1691,25 @@
     </row>
     <row r="12" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="6">
         <f>B8*B4/1000000</f>
         <v>2.7E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="6">
         <f>B8*B9*B10*B5</f>
@@ -904,19 +1731,792 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8D86EC-1095-A741-A8A1-C001B6DF60F6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="19" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="20">
+        <v>0.49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="21">
+        <v>476</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="C4" s="10">
+        <f>C3*730</f>
+        <v>357.7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="20">
+        <v>39.64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C5" s="6">
+        <f>B5*730*2</f>
+        <v>21.9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="22">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="23">
+        <f>Assumptions!C17</f>
+        <v>140000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14">
+        <f>Assumptions!C18</f>
+        <v>560000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15">
+        <f>(Assumptions!B17+Assumptions!B18)/15/3600</f>
+        <v>0.64814814814814814</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>22</v>
+      </c>
+      <c r="H15" s="27">
+        <f>E15*F15/24/30</f>
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17">
+        <f>B16*2</f>
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" ht="21" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="29">
+        <f>B12*C4*H15</f>
+        <v>491.83749999999992</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="27">
+        <f>H15</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="29">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="27"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="6">
+        <f>B16*C7*B12</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="6">
+        <f>B17*C9</f>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="7">
+        <f>SUM(B21:B27)</f>
+        <v>501.2374999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{3DE90303-8EFC-D14C-BF3A-2C8C1102D0BC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF301BF4-368D-B54D-A66D-0E57EBEC42C2}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection sqref="A1:B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="18">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="18"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="24">
+        <v>1.6</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
+        <v>6.1</v>
+      </c>
+      <c r="B12" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="24">
+        <v>13.5</v>
+      </c>
+      <c r="B13" s="18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="24">
+        <v>28.4</v>
+      </c>
+      <c r="B14" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="24">
+        <v>58.2</v>
+      </c>
+      <c r="B15" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="24">
+        <v>118</v>
+      </c>
+      <c r="B16" s="18">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="24">
+        <v>237</v>
+      </c>
+      <c r="B17" s="18">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="18">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="17">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="17">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="17">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="17">
+        <v>47.68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="25"/>
+      <c r="B30" s="17"/>
+    </row>
+    <row r="31" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="13"/>
+    </row>
+    <row r="32" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="18">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="18">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="18">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="19">
+        <v>51.31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA99E88E-191E-4E45-867C-2DFD74F16008}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="14">
+        <v>6.4999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1.2999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="17">
+        <f>Assumptions!C18</f>
+        <v>560000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="17">
+        <f>Assumptions!C19</f>
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="17">
+        <f>Assumptions!B9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="17">
+        <f>B12*B14/1024/1024</f>
+        <v>2.6702880859375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="17">
+        <f>ROUNDUP(ROUNDUP(B14/4,0)*B13/30/24/3600,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="17">
+        <f>ROUNDUP(B14*B13/24/30/3600,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="18">
+        <f>B4*B17*24*20</f>
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="6">
+        <f>B16*B5*24*20</f>
+        <v>6.239999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="6">
+        <f>B7*B15</f>
+        <v>0.5340576171875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="6">
+        <f>B15*B6</f>
+        <v>0.667572021484375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="7">
+        <f>SUM(B21:B24)</f>
+        <v>1.5760296386718751</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
made tenant manager basic
</commit_message>
<xml_diff>
--- a/docs/pricing-model.xlsx
+++ b/docs/pricing-model.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boyerje/Documents/Code/AWS/big-data-tenant-analytics/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE9DE93-95E7-4145-BFF8-A381E9743C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B409A-A669-9E40-B4EE-A985563873B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="500" windowWidth="29460" windowHeight="10360" activeTab="1" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
+    <workbookView xWindow="1740" yWindow="4120" windowWidth="30760" windowHeight="14320" activeTab="1" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
     <sheet name="S3" sheetId="7" r:id="rId2"/>
-    <sheet name="EKS" sheetId="8" r:id="rId3"/>
-    <sheet name="GuardDuty" sheetId="2" r:id="rId4"/>
-    <sheet name="Lambda" sheetId="3" r:id="rId5"/>
-    <sheet name="RDS-Postgresql" sheetId="4" r:id="rId6"/>
-    <sheet name="API Gateway" sheetId="6" r:id="rId7"/>
-    <sheet name="DynamoDB" sheetId="5" r:id="rId8"/>
+    <sheet name="SageMaker" sheetId="9" r:id="rId3"/>
+    <sheet name="EKS" sheetId="8" r:id="rId4"/>
+    <sheet name="GuardDuty" sheetId="2" r:id="rId5"/>
+    <sheet name="Lambda" sheetId="3" r:id="rId6"/>
+    <sheet name="RDS-Postgresql" sheetId="4" r:id="rId7"/>
+    <sheet name="API Gateway" sheetId="6" r:id="rId8"/>
+    <sheet name="DynamoDB" sheetId="5" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="170">
   <si>
     <t>nb-of-tenants</t>
   </si>
@@ -448,6 +449,108 @@
   </si>
   <si>
     <t>TB / month</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>Storage for SaaS execution analytics</t>
+  </si>
+  <si>
+    <t>Data for SaaS execution analytics</t>
+  </si>
+  <si>
+    <t>Storage for Tenant data</t>
+  </si>
+  <si>
+    <t>Storage for SaaS business</t>
+  </si>
+  <si>
+    <t>Cost Points</t>
+  </si>
+  <si>
+    <t>ml-t3..medium</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>ml.m5.xlarge</t>
+  </si>
+  <si>
+    <t>2 cCPU- 4GB</t>
+  </si>
+  <si>
+    <t>4 vCPU- 16GB</t>
+  </si>
+  <si>
+    <t>SageMaker Studio</t>
+  </si>
+  <si>
+    <t>SageMaker Studio Notebook</t>
+  </si>
+  <si>
+    <t>Runtime for model serving</t>
+  </si>
+  <si>
+    <t>ml.c5.xlarge</t>
+  </si>
+  <si>
+    <t>4 vCPU, 8 GB</t>
+  </si>
+  <si>
+    <t>24/7</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>ml.m5.4xlarge</t>
+  </si>
+  <si>
+    <t>16vCPU-32GB</t>
+  </si>
+  <si>
+    <t>ml.m5.4xlarge. - 5 minutes a day</t>
+  </si>
+  <si>
+    <t>Data out per day</t>
+  </si>
+  <si>
+    <t>Data in per day (MB)</t>
+  </si>
+  <si>
+    <t>Data process in / out</t>
+  </si>
+  <si>
+    <t>per GB</t>
+  </si>
+  <si>
+    <t>Infered dimensions</t>
+  </si>
+  <si>
+    <t>Data in and out</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>pricing</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Total per month</t>
   </si>
 </sst>
 </file>
@@ -459,9 +562,9 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0000_);[Red]\(&quot;$&quot;#,##0.0000\)"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -638,7 +741,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
@@ -655,15 +758,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -671,7 +774,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -680,7 +783,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="5" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1001,17 +1110,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34F96F2-6121-1F44-9B56-6D7ABA1B499B}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1116,6 +1226,13 @@
       <c r="C9" t="s">
         <v>32</v>
       </c>
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9">
+        <f>B9*B5*B4</f>
+        <v>67500</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
@@ -1129,148 +1246,171 @@
         <v>78</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <f>$B$4/2*$B$5</f>
+        <v>6750</v>
+      </c>
+      <c r="C13">
+        <f>B13*20</f>
+        <v>135000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <f>B13+B3/2</f>
+        <v>7000</v>
+      </c>
+      <c r="C14">
+        <f>B14*20</f>
+        <v>140000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <f>B14*4</f>
+        <v>28000</v>
+      </c>
+      <c r="C15">
+        <f>B15*20</f>
+        <v>560000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B16">
-        <f>$B$4/2*$B$5</f>
-        <v>6750</v>
+        <f>$B$4/2*$B$5*2</f>
+        <v>13500</v>
       </c>
       <c r="C16">
         <f>B16*20</f>
-        <v>135000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>270000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17">
-        <f>B16+B3/2</f>
-        <v>7000</v>
-      </c>
-      <c r="C17">
-        <f>B17*20</f>
-        <v>140000</v>
-      </c>
-      <c r="E17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18">
-        <f>B17*4</f>
-        <v>28000</v>
-      </c>
-      <c r="C18">
-        <f>B18*20</f>
-        <v>560000</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
         <v>54</v>
       </c>
-      <c r="B19">
-        <f>$B$4/2*$B$5*2</f>
-        <v>13500</v>
-      </c>
-      <c r="C19">
-        <f>B19*20</f>
-        <v>270000</v>
-      </c>
-      <c r="E19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B21" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B23" s="10">
+        <f>SageMaker!C23</f>
+        <v>305.86762249999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B24" s="10">
         <f>Lambda!B15</f>
         <v>5.0905125000000009</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B25" s="10">
         <f>'RDS-Postgresql'!B28</f>
         <v>501.2374999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B27" s="10">
+        <f>'S3'!B20</f>
+        <v>1.9315</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B31" s="10">
         <f>DynamoDB!B25</f>
         <v>1.5760296386718751</v>
       </c>
     </row>
+    <row r="34" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" s="33">
+        <f>SUM(B22:B32)</f>
+        <v>815.70316463867175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1278,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D75016-8D7E-6241-A9EC-C6A4879139F1}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1343,11 +1483,22 @@
         <v>131</v>
       </c>
       <c r="B11">
-        <f>Assumptions!B10</f>
-        <v>85000</v>
+        <f>Assumptions!B10/1000</f>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -1357,23 +1508,262 @@
     </row>
     <row r="17" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17">
-        <f>(B11-50000)</f>
-        <v>35000</v>
-      </c>
-    </row>
+        <v>139</v>
+      </c>
+      <c r="B17" s="10">
+        <f>(B11-50)*$B$5+50*$B$4</f>
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="10">
+        <f>B12*B4</f>
+        <v>1.15E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <f>SUM(B17:B19)</f>
+        <v>1.9315</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9903079B-0D9B-DE45-80BB-D0E322BED5EB}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0.05</v>
+      </c>
+      <c r="E4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="E6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="22">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="22">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="34">
+        <f>31*24</f>
+        <v>744</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="34">
+        <f>31*0.08</f>
+        <v>2.48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+      <c r="C15" s="34">
+        <f>31</f>
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" s="32"/>
+    </row>
+    <row r="19" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="6">
+        <f>B13*C13*C9</f>
+        <v>303.55199999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="6">
+        <f>B14*C6*C14</f>
+        <v>2.2865600000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="32">
+        <f>(B15+B16)*C10*C15/1024</f>
+        <v>2.9062499999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="7">
+        <f>SUM(C18:C22)</f>
+        <v>305.86762249999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{CEA92754-3AE2-884A-9F42-B761B1B91F07}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C681A54-95E7-4345-B314-53EA192E29AF}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
@@ -1591,7 +1981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4E1C13-7392-0E41-A5F4-7D1FC3F71AD2}">
   <dimension ref="A3"/>
   <sheetViews>
@@ -1614,7 +2004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098A98AF-AD43-C846-A6AB-538EEBD2CE08}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -1669,7 +2059,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="5">
-        <f>Assumptions!C16</f>
+        <f>Assumptions!C13</f>
         <v>135000</v>
       </c>
     </row>
@@ -1731,11 +2121,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8D86EC-1095-A741-A8A1-C001B6DF60F6}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -1871,7 +2261,7 @@
         <v>71</v>
       </c>
       <c r="B13" s="23">
-        <f>Assumptions!C17</f>
+        <f>Assumptions!C14</f>
         <v>140000</v>
       </c>
       <c r="C13" t="s">
@@ -1883,7 +2273,7 @@
         <v>72</v>
       </c>
       <c r="B14">
-        <f>Assumptions!C18</f>
+        <f>Assumptions!C15</f>
         <v>560000</v>
       </c>
       <c r="C14" t="s">
@@ -1904,7 +2294,7 @@
         <v>73</v>
       </c>
       <c r="B15">
-        <f>(Assumptions!B17+Assumptions!B18)/15/3600</f>
+        <f>(Assumptions!B14+Assumptions!B15)/15/3600</f>
         <v>0.64814814814814814</v>
       </c>
       <c r="C15" t="s">
@@ -2032,7 +2422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF301BF4-368D-B54D-A66D-0E57EBEC42C2}">
   <dimension ref="A1:B37"/>
   <sheetViews>
@@ -2317,7 +2707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA99E88E-191E-4E45-867C-2DFD74F16008}">
   <dimension ref="A1:B26"/>
   <sheetViews>
@@ -2410,7 +2800,7 @@
         <v>43</v>
       </c>
       <c r="B12" s="17">
-        <f>Assumptions!C18</f>
+        <f>Assumptions!C15</f>
         <v>560000</v>
       </c>
     </row>
@@ -2419,7 +2809,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="17">
-        <f>Assumptions!C19</f>
+        <f>Assumptions!C16</f>
         <v>270000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add update to kinesis doc and api gtw
</commit_message>
<xml_diff>
--- a/docs/pricing-model.xlsx
+++ b/docs/pricing-model.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boyerje/Documents/Code/AWS/big-data-tenant-analytics/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375B409A-A669-9E40-B4EE-A985563873B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BD4EE0-6FF4-5245-9CC4-B53329A21A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="4120" windowWidth="30760" windowHeight="14320" activeTab="1" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
+    <workbookView xWindow="46960" yWindow="2360" windowWidth="24420" windowHeight="17960" activeTab="1" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
-    <sheet name="S3" sheetId="7" r:id="rId2"/>
-    <sheet name="SageMaker" sheetId="9" r:id="rId3"/>
-    <sheet name="EKS" sheetId="8" r:id="rId4"/>
-    <sheet name="GuardDuty" sheetId="2" r:id="rId5"/>
-    <sheet name="Lambda" sheetId="3" r:id="rId6"/>
-    <sheet name="RDS-Postgresql" sheetId="4" r:id="rId7"/>
-    <sheet name="API Gateway" sheetId="6" r:id="rId8"/>
-    <sheet name="DynamoDB" sheetId="5" r:id="rId9"/>
+    <sheet name="Kinesis" sheetId="11" r:id="rId2"/>
+    <sheet name="S3" sheetId="7" r:id="rId3"/>
+    <sheet name="SageMaker" sheetId="9" r:id="rId4"/>
+    <sheet name="EKS" sheetId="8" r:id="rId5"/>
+    <sheet name="GuardDuty" sheetId="2" r:id="rId6"/>
+    <sheet name="Lambda" sheetId="3" r:id="rId7"/>
+    <sheet name="RDS-Postgresql" sheetId="4" r:id="rId8"/>
+    <sheet name="API Gateway" sheetId="6" r:id="rId9"/>
+    <sheet name="QuickSight" sheetId="10" r:id="rId10"/>
+    <sheet name="DynamoDB" sheetId="5" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="222">
   <si>
     <t>nb-of-tenants</t>
   </si>
@@ -121,15 +123,6 @@
     <t>S3</t>
   </si>
   <si>
-    <t>Glacier</t>
-  </si>
-  <si>
-    <t>IAM</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
     <t>Assumptions: Big Data analytics job during week day done by analytics, scientists..For a SaaS company adding rt-analytiics on metadata events</t>
   </si>
   <si>
@@ -223,9 +216,6 @@
     <t>nb-of-job/day/developer</t>
   </si>
   <si>
-    <t>nb-of-user-developer overall</t>
-  </si>
-  <si>
     <t>RDS</t>
   </si>
   <si>
@@ -551,13 +541,181 @@
   </si>
   <si>
     <t>Total per month</t>
+  </si>
+  <si>
+    <t>persons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Cost points	</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>authors</t>
+  </si>
+  <si>
+    <t>authors with Q capability</t>
+  </si>
+  <si>
+    <t>Authors with Q</t>
+  </si>
+  <si>
+    <t>readers</t>
+  </si>
+  <si>
+    <t>readers with Q</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>Session in average</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Capacity pricing</t>
+  </si>
+  <si>
+    <t>Capacity Q base</t>
+  </si>
+  <si>
+    <t>500 sessions</t>
+  </si>
+  <si>
+    <t>Paginated Report</t>
+  </si>
+  <si>
+    <t>500 month</t>
+  </si>
+  <si>
+    <t>Spice</t>
+  </si>
+  <si>
+    <t>30 minutes session</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>Reader session based</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Expected data size</t>
+  </si>
+  <si>
+    <t>GB / month</t>
+  </si>
+  <si>
+    <t>report  including email</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Kinesis</t>
+  </si>
+  <si>
+    <t>Glacier deep archive</t>
+  </si>
+  <si>
+    <t>Glacier instant retrieval</t>
+  </si>
+  <si>
+    <t>Archive</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>1 MB/second of write and 2 MB/second of read throughout.</t>
+  </si>
+  <si>
+    <t>Shard hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data retention </t>
+  </si>
+  <si>
+    <t># Shard</t>
+  </si>
+  <si>
+    <t>Retention</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>Message Size</t>
+  </si>
+  <si>
+    <t>Used for metadata analytics</t>
+  </si>
+  <si>
+    <t>for 7 days</t>
+  </si>
+  <si>
+    <t>GB in a year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DynamoDB Read ops </t>
+  </si>
+  <si>
+    <t>Shard</t>
+  </si>
+  <si>
+    <t>nb-of-user-developer cross tenant</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>Data produced</t>
+  </si>
+  <si>
+    <t>For simplicity, we assume that the throughput and data size of each record are stable and constant throughout the day</t>
+  </si>
+  <si>
+    <t>Throughput /s</t>
+  </si>
+  <si>
+    <t>MB/s</t>
+  </si>
+  <si>
+    <t>PUT Payload Unit </t>
+  </si>
+  <si>
+    <t>of 25k</t>
+  </si>
+  <si>
+    <t>Put Payload unit /s</t>
+  </si>
+  <si>
+    <t>per 1 million of unit per month. 25k of data</t>
+  </si>
+  <si>
+    <t>PUT Payload Unit (25k)</t>
+  </si>
+  <si>
+    <t>msg per second</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -565,8 +723,9 @@
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -668,6 +827,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -741,7 +932,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
@@ -786,10 +977,17 @@
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="5" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1110,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34F96F2-6121-1F44-9B56-6D7ABA1B499B}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1324,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -1144,25 +1342,25 @@
         <v>500</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
       <c r="B4">
         <f>B3*10</f>
         <v>5000</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D4">
         <v>1.7</v>
@@ -1170,13 +1368,13 @@
     </row>
     <row r="5" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B5" s="8">
         <v>2.7</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <f>2*B5</f>
@@ -1218,16 +1416,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" s="8">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E9">
         <f>B9*B5*B4</f>
@@ -1236,19 +1434,19 @@
     </row>
     <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B10" s="8">
         <f>B3*D3*D4</f>
         <v>85000</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>18</v>
@@ -1259,7 +1457,7 @@
     </row>
     <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <f>$B$4/2*$B$5</f>
@@ -1272,7 +1470,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <f>B13+B3/2</f>
@@ -1283,12 +1481,12 @@
         <v>140000</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <f>B14*4</f>
@@ -1299,12 +1497,12 @@
         <v>560000</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <f>$B$4/2*$B$5*2</f>
@@ -1315,12 +1513,12 @@
         <v>270000</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -1328,13 +1526,17 @@
         <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>3</v>
       </c>
+      <c r="B22" s="10">
+        <f>QuickSight!B27</f>
+        <v>779.4</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1356,7 +1558,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B25" s="10">
         <f>'RDS-Postgresql'!B28</f>
@@ -1367,6 +1569,10 @@
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="B26" s="10">
+        <f>EKS!B28</f>
+        <v>296.27999999999997</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1374,59 +1580,724 @@
       </c>
       <c r="B27" s="10">
         <f>'S3'!B20</f>
-        <v>1.9315</v>
+        <v>10.0715</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
+      <c r="B28" s="10"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>193</v>
+      </c>
+      <c r="B29" s="6">
+        <f>Kinesis!B26</f>
+        <v>32.142650000000003</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="10">
+        <v>33</v>
+      </c>
+      <c r="B30" s="10">
         <f>DynamoDB!B25</f>
         <v>1.5760296386718751</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+    <row r="35" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B35" s="33">
+        <f>SUM(B22:B33)</f>
+        <v>1931.6658146386717</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BAAB45-49E0-FB43-A441-319A25A53D81}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B34" s="33">
-        <f>SUM(B22:B32)</f>
-        <v>815.70316463867175</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="6">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="6">
+        <v>34</v>
+      </c>
+      <c r="C4" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="6">
+        <v>250</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" s="6">
+        <v>250</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="6">
+        <v>500</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <v>500</v>
+      </c>
+      <c r="C17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19">
+        <v>500</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="10">
+        <f>B14*B4</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23" s="10">
+        <f>E8*B16+B15*E7</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>187</v>
+      </c>
+      <c r="B24" s="10">
+        <f>B9</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="10">
+        <f>B18*B10</f>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B27" s="10">
+        <f>SUM(B22:B25)</f>
+        <v>779.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA99E88E-191E-4E45-867C-2DFD74F16008}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="14">
+        <v>6.4999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1.2999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="15">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13"/>
+    </row>
+    <row r="12" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="17">
+        <f>Assumptions!C15</f>
+        <v>560000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="17">
+        <f>Assumptions!C16</f>
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="17">
+        <f>Assumptions!B9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="17">
+        <f>B12*B14/1024/1024</f>
+        <v>2.6702880859375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="17">
+        <f>ROUNDUP(ROUNDUP(B14/4,0)*B13/30/24/3600,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="17">
+        <f>ROUNDUP(B14*B13/24/30/3600,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="13"/>
+    </row>
+    <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="18">
+        <f>B4*B17*24*20</f>
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="6">
+        <f>B16*B5*24*20</f>
+        <v>6.239999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="6">
+        <f>B7*B15</f>
+        <v>0.5340576171875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="6">
+        <f>B15*B6</f>
+        <v>0.667572021484375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="7">
+        <f>SUM(B21:B24)</f>
+        <v>1.5760296386718751</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DBEC21-EDFB-5648-8FCE-9EA715245714}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="53.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="41">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="41">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="22">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="37"/>
+    </row>
+    <row r="10" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14">
+        <f>ROUNDUP(B15/25,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="8">
+        <f>Assumptions!B9</f>
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="8">
+        <f>Assumptions!B4*Assumptions!B5*2/B13/3600</f>
+        <v>0.75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" s="42">
+        <f>B16*B15/1024</f>
+        <v>3.662109375E-3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>209</v>
+      </c>
+      <c r="B20" s="10">
+        <f>B4*24*31</f>
+        <v>13.540800000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" s="41">
+        <f>ROUND(B14*3600*31/1000000,1)*B5</f>
+        <v>1.8500000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B22" s="6">
+        <f>B11*24*31*B6</f>
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="7">
+        <f>SUM(B20:B25)</f>
+        <v>32.142650000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D75016-8D7E-6241-A9EC-C6A4879139F1}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
@@ -1443,91 +2314,139 @@
       <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="13"/>
+      <c r="B3" s="13" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="18" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B4" s="31">
         <v>2.3E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5">
+        <v>129</v>
+      </c>
+      <c r="B5" s="22">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6">
+        <v>128</v>
+      </c>
+      <c r="B6" s="22">
         <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="36">
+        <v>9.8999999999999999E-4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B11">
-        <f>Assumptions!B10/1000</f>
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B12">
         <v>0.5</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B16" s="13" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="17" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B17" s="10">
         <f>(B11-50)*$B$5+50*$B$4</f>
-        <v>1.92</v>
+        <v>0.15999999999999992</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B18" s="10">
         <f>B12*B4</f>
         <v>1.15E-2</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="10">
+        <f>B13*1000*B8</f>
+        <v>9.9</v>
+      </c>
+    </row>
     <row r="20" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <f>SUM(B17:B19)</f>
-        <v>1.9315</v>
+        <v>10.0715</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
@@ -1536,7 +2455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9903079B-0D9B-DE45-80BB-D0E322BED5EB}">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -1553,90 +2472,90 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="22">
         <v>0.05</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" s="22">
         <v>0.23</v>
       </c>
       <c r="E5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C6" s="22">
         <v>0.92200000000000004</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C9" s="22">
         <v>0.20399999999999999</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C10" s="22">
         <v>1.6E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -1644,66 +2563,66 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" s="34">
+      <c r="C13">
         <f>31*24</f>
         <v>744</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="34">
+      <c r="C14">
         <f>31*0.08</f>
         <v>2.48</v>
       </c>
       <c r="D14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B15">
         <v>50</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15">
         <f>31</f>
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -1719,7 +2638,7 @@
     </row>
     <row r="20" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C20" s="6">
         <f>B13*C13*C9</f>
@@ -1728,7 +2647,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C21" s="6">
         <f>B14*C6*C14</f>
@@ -1737,7 +2656,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C22" s="32">
         <f>(B15+B16)*C10*C15/1024</f>
@@ -1759,7 +2678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C681A54-95E7-4345-B314-53EA192E29AF}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -1775,7 +2694,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -1791,7 +2710,7 @@
     </row>
     <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B4" s="18">
         <v>0.15</v>
@@ -1799,7 +2718,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B5" s="18">
         <v>0.2</v>
@@ -1807,7 +2726,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B6" s="18">
         <v>0.02</v>
@@ -1815,7 +2734,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B7" s="18">
         <v>0.01</v>
@@ -1823,7 +2742,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B8" s="18">
         <v>0.1</v>
@@ -1841,7 +2760,7 @@
     </row>
     <row r="11" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B11" s="17">
         <v>8000000</v>
@@ -1849,7 +2768,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B12" s="12">
         <v>0.25</v>
@@ -1857,7 +2776,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B13" s="17">
         <v>3.09</v>
@@ -1865,7 +2784,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B14" s="17">
         <v>3.09</v>
@@ -1873,7 +2792,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B15" s="17">
         <v>30.86</v>
@@ -1881,7 +2800,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B16" s="17">
         <v>23.15</v>
@@ -1889,7 +2808,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B17" s="17">
         <v>5.79</v>
@@ -1897,7 +2816,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B18" s="17">
         <v>100</v>
@@ -1905,7 +2824,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B19" s="17">
         <v>8</v>
@@ -1913,7 +2832,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B20" s="17">
         <v>32</v>
@@ -1921,7 +2840,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B21" s="17">
         <v>1</v>
@@ -1939,7 +2858,7 @@
     </row>
     <row r="24" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B24" s="18">
         <v>108.3</v>
@@ -1947,7 +2866,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B25" s="18">
         <v>144</v>
@@ -1955,7 +2874,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B26" s="18">
         <v>33.979999999999997</v>
@@ -1963,7 +2882,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B27" s="18">
         <v>10</v>
@@ -1981,7 +2900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4E1C13-7392-0E41-A5F4-7D1FC3F71AD2}">
   <dimension ref="A3"/>
   <sheetViews>
@@ -2004,7 +2923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098A98AF-AD43-C846-A6AB-538EEBD2CE08}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -2023,7 +2942,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -2094,7 +3013,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2121,7 +3040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8D86EC-1095-A741-A8A1-C001B6DF60F6}">
   <dimension ref="A1:H29"/>
   <sheetViews>
@@ -2139,10 +3058,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -2151,32 +3070,32 @@
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C3" s="20">
         <v>0.49</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E3" s="21">
         <v>476</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
@@ -2196,7 +3115,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>1.4999999999999999E-2</v>
@@ -2211,35 +3130,35 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C7" s="22">
         <v>0.25</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C8" s="22">
         <v>0.2</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C9" s="22">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -2250,7 +3169,7 @@
     </row>
     <row r="12" spans="1:8" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B12" s="26">
         <v>3</v>
@@ -2258,7 +3177,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B13" s="23">
         <f>Assumptions!C14</f>
@@ -2270,7 +3189,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B14">
         <f>Assumptions!C15</f>
@@ -2280,25 +3199,25 @@
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B15">
         <f>(Assumptions!B14+Assumptions!B15)/15/3600</f>
         <v>0.64814814814814814</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -2313,25 +3232,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B16">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B17">
         <f>B16*2</f>
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
@@ -2342,26 +3261,26 @@
     </row>
     <row r="21" spans="1:5" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B21" s="29">
         <f>B12*C4*H15</f>
         <v>491.83749999999992</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D21" s="27">
         <f>H15</f>
         <v>0.45833333333333331</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B22" s="29">
         <f>0</f>
@@ -2372,25 +3291,25 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B23" s="18"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B26" s="6">
         <f>B16*C7*B12</f>
@@ -2399,7 +3318,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B27" s="6">
         <f>B17*C9</f>
@@ -2422,7 +3341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF301BF4-368D-B54D-A66D-0E57EBEC42C2}">
   <dimension ref="A1:B37"/>
   <sheetViews>
@@ -2438,7 +3357,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -2454,13 +3373,13 @@
     </row>
     <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B5" s="18">
         <v>3.5</v>
@@ -2468,7 +3387,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" s="18">
         <v>2.8</v>
@@ -2476,7 +3395,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B7" s="18">
         <v>2.38</v>
@@ -2484,7 +3403,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B8" s="18">
         <v>1.51</v>
@@ -2492,7 +3411,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B9" s="18"/>
     </row>
@@ -2562,7 +3481,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B18" s="18">
         <v>0.02</v>
@@ -2580,7 +3499,7 @@
     </row>
     <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B21" s="17">
         <v>10000000</v>
@@ -2588,7 +3507,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B22" s="17">
         <v>10000000</v>
@@ -2596,31 +3515,31 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26" s="17">
         <v>0.01</v>
@@ -2628,7 +3547,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B27" s="17">
         <v>0.5</v>
@@ -2636,7 +3555,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B28" s="17">
         <v>0.02</v>
@@ -2644,7 +3563,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B29" s="17">
         <v>47.68</v>
@@ -2662,7 +3581,7 @@
     </row>
     <row r="32" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B32" s="18">
         <v>35</v>
@@ -2670,7 +3589,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B33" s="18">
         <v>14.4</v>
@@ -2678,7 +3597,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B34" s="18">
         <v>0.95</v>
@@ -2686,7 +3605,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B35" s="18">
         <v>0.95</v>
@@ -2705,209 +3624,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA99E88E-191E-4E45-867C-2DFD74F16008}">
-  <dimension ref="A1:B26"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="12"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-    </row>
-    <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="13"/>
-    </row>
-    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="14">
-        <v>6.4999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="14">
-        <v>1.2999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="15">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="15">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="15">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13"/>
-    </row>
-    <row r="12" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="17">
-        <f>Assumptions!C15</f>
-        <v>560000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="17">
-        <f>Assumptions!C16</f>
-        <v>270000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="17">
-        <f>Assumptions!B9</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="17">
-        <f>B12*B14/1024/1024</f>
-        <v>2.6702880859375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="17">
-        <f>ROUNDUP(ROUNDUP(B14/4,0)*B13/30/24/3600,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="17">
-        <f>ROUNDUP(B14*B13/24/30/3600,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="17"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="13"/>
-    </row>
-    <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="18">
-        <f>B4*B17*24*20</f>
-        <v>0.312</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="6">
-        <f>B16*B5*24*20</f>
-        <v>6.239999999999999E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="6">
-        <f>B7*B15</f>
-        <v>0.5340576171875</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="6">
-        <f>B15*B6</f>
-        <v>0.667572021484375</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="7">
-        <f>SUM(B21:B24)</f>
-        <v>1.5760296386718751</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
work on improving flink processing
</commit_message>
<xml_diff>
--- a/docs/pricing-model.xlsx
+++ b/docs/pricing-model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boyerje/Documents/Code/AWS/big-data-tenant-analytics/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BD4EE0-6FF4-5245-9CC4-B53329A21A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3CCCA2-3303-E048-B3EF-E755AE4BB1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46960" yWindow="2360" windowWidth="24420" windowHeight="17960" activeTab="1" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
+    <workbookView xWindow="46960" yWindow="2360" windowWidth="24420" windowHeight="17960" xr2:uid="{D425A971-54F1-3144-B2A7-8B3877C84570}"/>
   </bookViews>
   <sheets>
     <sheet name="Assumptions" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="227">
   <si>
     <t>nb-of-tenants</t>
   </si>
@@ -51,9 +51,6 @@
     <t>MB</t>
   </si>
   <si>
-    <t>Summary</t>
-  </si>
-  <si>
     <t>QuickSight</t>
   </si>
   <si>
@@ -709,6 +706,24 @@
   </si>
   <si>
     <t>msg per second</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Compute</t>
   </si>
 </sst>
 </file>
@@ -725,7 +740,7 @@
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -859,6 +874,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -932,7 +961,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
@@ -988,6 +1017,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1308,312 +1339,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34F96F2-6121-1F44-9B56-6D7ABA1B499B}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="B1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>500</v>
+      </c>
+      <c r="E3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4">
+        <f>D3*10</f>
+        <v>5000</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8">
-        <v>500</v>
-      </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>210</v>
-      </c>
-      <c r="B4">
-        <f>B3*10</f>
-        <v>5000</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="8">
-        <v>2.7</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5">
-        <f>2*B5</f>
+      <c r="G5">
+        <f>2*D5</f>
         <v>5.4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8">
         <v>1000</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="8">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="8">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D8" s="8">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="8">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9">
-        <f>B9*B5*B4</f>
+      <c r="F9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9">
+        <f>D9*D5*D4</f>
         <v>67500</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="8">
-        <f>B3*D3*D4</f>
+    <row r="10" spans="3:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="C10" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="8">
+        <f>D3*F3*F4</f>
         <v>85000</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13">
+        <f>$D$4/2*$D$5</f>
+        <v>6750</v>
+      </c>
+      <c r="E13">
+        <f>D13*20</f>
+        <v>135000</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14">
+        <f>D13+D3/2</f>
+        <v>7000</v>
+      </c>
+      <c r="E14">
+        <f>D14*20</f>
+        <v>140000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15">
+        <f>D14*4</f>
+        <v>28000</v>
+      </c>
+      <c r="E15">
+        <f>D15*20</f>
+        <v>560000</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <f>$D$4/2*$D$5*2</f>
+        <v>13500</v>
+      </c>
+      <c r="E16">
+        <f>D16*20</f>
+        <v>270000</v>
+      </c>
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13">
-        <f>$B$4/2*$B$5</f>
-        <v>6750</v>
-      </c>
-      <c r="C13">
-        <f>B13*20</f>
-        <v>135000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14">
-        <f>B13+B3/2</f>
-        <v>7000</v>
-      </c>
-      <c r="C14">
-        <f>B14*20</f>
-        <v>140000</v>
-      </c>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15">
-        <f>B14*4</f>
-        <v>28000</v>
-      </c>
-      <c r="C15">
-        <f>B15*20</f>
-        <v>560000</v>
-      </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16">
-        <f>$B$4/2*$B$5*2</f>
-        <v>13500</v>
-      </c>
-      <c r="C16">
-        <f>B16*20</f>
-        <v>270000</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="10">
+      <c r="D22" s="10">
         <f>QuickSight!B27</f>
         <v>779.4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="10">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="10">
         <f>SageMaker!C23</f>
         <v>305.86762249999998</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="10">
-        <f>Lambda!B15</f>
-        <v>5.0905125000000009</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="10">
-        <f>'RDS-Postgresql'!B28</f>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="10">
+        <f>'RDS-Postgresql'!$B$28</f>
         <v>501.2374999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="10">
+        <f>DynamoDB!$B$25</f>
+        <v>1.5760296386718751</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="10">
-        <f>EKS!B28</f>
-        <v>296.27999999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="10">
+      <c r="D27" s="10">
         <f>'S3'!B20</f>
         <v>10.0715</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="10"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="6">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="10">
+        <f>Lambda!$B$15</f>
+        <v>5.0905125000000009</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>192</v>
+      </c>
+      <c r="D29" s="6">
         <f>Kinesis!B26</f>
         <v>32.142650000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="10">
-        <f>DynamoDB!B25</f>
-        <v>1.5760296386718751</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="B35" s="33">
-        <f>SUM(B22:B33)</f>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="10">
+        <f>EKS!$B$28</f>
+        <v>296.27999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" s="33">
+        <f>SUM(D22:D33)</f>
         <v>1931.6658146386717</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="3:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1636,23 +1680,23 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="6">
         <v>24</v>
@@ -1663,7 +1707,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="6">
         <v>34</v>
@@ -1674,39 +1718,39 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="6">
         <v>0.3</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="6">
         <v>0.3</v>
       </c>
       <c r="E6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="6">
         <v>250</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="6">
         <v>5</v>
@@ -1714,14 +1758,14 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" s="6">
         <v>250</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E8" s="6">
         <v>10</v>
@@ -1729,31 +1773,31 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B9" s="6">
         <v>500</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="6">
         <v>0.38</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1761,18 +1805,18 @@
     <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -1780,7 +1824,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -1788,47 +1832,47 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17">
         <v>500</v>
       </c>
       <c r="C17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B18">
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B19">
         <v>500</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" s="10">
         <f>B14*B4</f>
@@ -1837,7 +1881,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B23" s="10">
         <f>E8*B16+B15*E7</f>
@@ -1846,7 +1890,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B24" s="10">
         <f>B9</f>
@@ -1855,7 +1899,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="10">
         <f>B18*B10</f>
@@ -1864,7 +1908,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B27" s="10">
         <f>SUM(B22:B25)</f>
@@ -1892,7 +1936,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -1902,13 +1946,13 @@
     </row>
     <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="14">
         <v>6.4999999999999997E-4</v>
@@ -1916,7 +1960,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="14">
         <v>1.2999999999999999E-4</v>
@@ -1924,7 +1968,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="15">
         <v>0.25</v>
@@ -1932,7 +1976,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="15">
         <v>0.2</v>
@@ -1940,7 +1984,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="15">
         <v>1E-3</v>
@@ -1948,7 +1992,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="15">
         <v>0.02</v>
@@ -1960,40 +2004,40 @@
     </row>
     <row r="11" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="17">
-        <f>Assumptions!C15</f>
+        <f>Assumptions!E15</f>
         <v>560000</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="17">
-        <f>Assumptions!C16</f>
+        <f>Assumptions!E16</f>
         <v>270000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="17">
-        <f>Assumptions!B9</f>
+        <f>Assumptions!D9</f>
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="17">
         <f>B12*B14/1024/1024</f>
@@ -2002,7 +2046,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="17">
         <f>ROUNDUP(ROUNDUP(B14/4,0)*B13/30/24/3600,0)</f>
@@ -2011,7 +2055,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="17">
         <f>ROUNDUP(B14*B13/24/30/3600,0)</f>
@@ -2028,13 +2072,13 @@
     </row>
     <row r="20" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="13"/>
     </row>
     <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="18">
         <f>B4*B17*24*20</f>
@@ -2043,7 +2087,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="6">
         <f>B16*B5*24*20</f>
@@ -2052,7 +2096,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B23" s="6">
         <f>B7*B15</f>
@@ -2061,7 +2105,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="6">
         <f>B15*B6</f>
@@ -2085,7 +2129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DBEC21-EDFB-5648-8FCE-9EA715245714}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -2097,51 +2141,51 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="41">
         <v>1.8200000000000001E-2</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" s="41">
         <v>1.8499999999999999E-2</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="22">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2149,18 +2193,18 @@
     </row>
     <row r="10" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2168,85 +2212,85 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B14">
         <f>ROUNDUP(B15/25,0)</f>
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="8">
-        <f>Assumptions!B9</f>
+        <f>Assumptions!D9</f>
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B16" s="8">
-        <f>Assumptions!B4*Assumptions!B5*2/B13/3600</f>
+        <f>Assumptions!D4*Assumptions!D5*2/B13/3600</f>
         <v>0.75</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B17" s="42">
         <f>B16*B15/1024</f>
         <v>3.662109375E-3</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B20" s="10">
         <f>B4*24*31</f>
@@ -2255,7 +2299,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" s="41">
         <f>ROUND(B14*3600*31/1000000,1)*B5</f>
@@ -2264,7 +2308,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B22" s="6">
         <f>B11*24*31*B6</f>
@@ -2273,7 +2317,7 @@
     </row>
     <row r="26" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" s="7">
         <f>SUM(B20:B25)</f>
@@ -2302,7 +2346,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -2312,26 +2356,26 @@
     </row>
     <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="31">
         <v>2.3E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="22">
         <v>2.1999999999999999E-2</v>
@@ -2339,7 +2383,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="22">
         <v>2.1000000000000001E-2</v>
@@ -2347,78 +2391,78 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" s="22">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B8" s="36">
         <v>9.8999999999999999E-4</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12">
         <v>0.5</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="10">
         <f>(B11-50)*$B$5+50*$B$4</f>
@@ -2427,7 +2471,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" s="10">
         <f>B12*B4</f>
@@ -2436,7 +2480,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B19" s="10">
         <f>B13*1000*B8</f>
@@ -2472,106 +2516,106 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="22">
         <v>0.05</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="22">
         <v>0.23</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
         <v>149</v>
-      </c>
-      <c r="B6" t="s">
-        <v>150</v>
       </c>
       <c r="C6" s="22">
         <v>0.92200000000000004</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" t="s">
         <v>145</v>
-      </c>
-      <c r="B9" t="s">
-        <v>146</v>
       </c>
       <c r="C9" s="22">
         <v>0.20399999999999999</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" s="22">
         <v>1.6E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -2581,15 +2625,15 @@
         <v>744</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2599,15 +2643,15 @@
         <v>2.48</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B15">
         <v>50</v>
@@ -2617,12 +2661,12 @@
         <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16">
         <v>10</v>
@@ -2631,14 +2675,14 @@
     </row>
     <row r="19" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="6">
         <f>B13*C13*C9</f>
@@ -2647,7 +2691,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="6">
         <f>B14*C6*C14</f>
@@ -2656,7 +2700,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" s="32">
         <f>(B15+B16)*C10*C15/1024</f>
@@ -2694,7 +2738,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -2704,13 +2748,13 @@
     </row>
     <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="18">
         <v>0.15</v>
@@ -2718,7 +2762,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="18">
         <v>0.2</v>
@@ -2726,7 +2770,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="18">
         <v>0.02</v>
@@ -2734,7 +2778,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="18">
         <v>0.01</v>
@@ -2742,7 +2786,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="18">
         <v>0.1</v>
@@ -2754,13 +2798,13 @@
     </row>
     <row r="10" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="17">
         <v>8000000</v>
@@ -2768,7 +2812,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="12">
         <v>0.25</v>
@@ -2776,7 +2820,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="17">
         <v>3.09</v>
@@ -2784,7 +2828,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="17">
         <v>3.09</v>
@@ -2792,7 +2836,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15" s="17">
         <v>30.86</v>
@@ -2800,7 +2844,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B16" s="17">
         <v>23.15</v>
@@ -2808,7 +2852,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" s="17">
         <v>5.79</v>
@@ -2816,7 +2860,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B18" s="17">
         <v>100</v>
@@ -2824,7 +2868,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" s="17">
         <v>8</v>
@@ -2832,7 +2876,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20" s="17">
         <v>32</v>
@@ -2840,7 +2884,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" s="17">
         <v>1</v>
@@ -2852,13 +2896,13 @@
     </row>
     <row r="23" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="13"/>
     </row>
     <row r="24" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B24" s="18">
         <v>108.3</v>
@@ -2866,7 +2910,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B25" s="18">
         <v>144</v>
@@ -2874,7 +2918,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="18">
         <v>33.979999999999997</v>
@@ -2882,7 +2926,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B27" s="18">
         <v>10</v>
@@ -2912,7 +2956,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2939,21 +2983,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>0.2</v>
@@ -2961,7 +3005,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>1.6670000000000001E-5</v>
@@ -2969,22 +3013,22 @@
     </row>
     <row r="7" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5">
-        <f>Assumptions!C13</f>
+        <f>Assumptions!E13</f>
         <v>135000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2992,7 +3036,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0.75</v>
@@ -3000,25 +3044,25 @@
     </row>
     <row r="12" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="6">
         <f>B8*B4/1000000</f>
         <v>2.7E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="6">
         <f>B8*B9*B10*B5</f>
@@ -3058,44 +3102,44 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="19" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="20">
         <v>0.49</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="21">
         <v>476</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
@@ -3104,18 +3148,18 @@
         <v>357.7</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="20">
         <v>39.64</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>1.4999999999999999E-2</v>
@@ -3125,51 +3169,51 @@
         <v>21.9</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="22">
         <v>0.25</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="22">
         <v>0.2</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="22">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:8" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="26">
         <v>3</v>
@@ -3177,47 +3221,47 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="23">
-        <f>Assumptions!C14</f>
+        <f>Assumptions!E14</f>
         <v>140000</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14">
-        <f>Assumptions!C15</f>
+        <f>Assumptions!E15</f>
         <v>560000</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
         <v>71</v>
       </c>
-      <c r="F14" t="s">
-        <v>72</v>
-      </c>
       <c r="H14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15">
+        <f>(Assumptions!D14+Assumptions!D15)/15/3600</f>
+        <v>0.64814814814814814</v>
+      </c>
+      <c r="C15" t="s">
         <v>69</v>
-      </c>
-      <c r="B15">
-        <f>(Assumptions!B14+Assumptions!B15)/15/3600</f>
-        <v>0.64814814814814814</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
       </c>
       <c r="E15">
         <v>15</v>
@@ -3232,55 +3276,55 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <f>B16*2</f>
         <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="13"/>
     </row>
     <row r="21" spans="1:5" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="29">
         <f>B12*C4*H15</f>
         <v>491.83749999999992</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" s="27">
         <f>H15</f>
         <v>0.45833333333333331</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="29">
         <f>0</f>
@@ -3291,25 +3335,25 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="18"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="6">
         <f>B16*C7*B12</f>
@@ -3318,7 +3362,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" s="6">
         <f>B17*C9</f>
@@ -3357,7 +3401,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -3367,19 +3411,19 @@
     </row>
     <row r="3" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="13"/>
     </row>
     <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="18">
         <v>3.5</v>
@@ -3387,7 +3431,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="18">
         <v>2.8</v>
@@ -3395,7 +3439,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="18">
         <v>2.38</v>
@@ -3403,7 +3447,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="18">
         <v>1.51</v>
@@ -3411,7 +3455,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="18"/>
     </row>
@@ -3481,7 +3525,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="18">
         <v>0.02</v>
@@ -3493,13 +3537,13 @@
     </row>
     <row r="20" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="13"/>
     </row>
     <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="17">
         <v>10000000</v>
@@ -3507,7 +3551,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="17">
         <v>10000000</v>
@@ -3515,31 +3559,31 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="17">
         <v>0.01</v>
@@ -3547,7 +3591,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" s="17">
         <v>0.5</v>
@@ -3555,7 +3599,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="17">
         <v>0.02</v>
@@ -3563,7 +3607,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="17">
         <v>47.68</v>
@@ -3575,13 +3619,13 @@
     </row>
     <row r="31" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" s="13"/>
     </row>
     <row r="32" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="18">
         <v>35</v>
@@ -3589,7 +3633,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B33" s="18">
         <v>14.4</v>
@@ -3597,7 +3641,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B34" s="18">
         <v>0.95</v>
@@ -3605,7 +3649,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="18">
         <v>0.95</v>

</xml_diff>